<commit_message>
updating existing for 20.10
</commit_message>
<xml_diff>
--- a/Complete Word Template from Excel and Email/Project_Notebook.xlsx
+++ b/Complete Word Template from Excel and Email/Project_Notebook.xlsx
@@ -1,63 +1,64 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Studio\Studio\UiPath.Studio.Plugin.Workflow\ProjectTemplates\Business Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\studio\Studio\UiPath.Studio.Plugin.Workflow\ProjectTemplates\Business Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6BF730-1D91-4059-A4D7-3507558AA061}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65B5E3D-CC52-4BC8-BE61-079C0D7486C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{CEA043F9-B9CC-4A62-BD5F-6FF44D9B0F3D}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="23040" windowHeight="12204" xr2:uid="{CEA043F9-B9CC-4A62-BD5F-6FF44D9B0F3D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Scratchpad" sheetId="2" r:id="rId1"/>
+    <sheet name="About the Project Notebook" sheetId="2" r:id="rId1"/>
     <sheet name="Date" sheetId="1" r:id="rId2"/>
     <sheet name="Text" sheetId="3" r:id="rId3"/>
     <sheet name="Number" sheetId="4" r:id="rId4"/>
     <sheet name="File" sheetId="5" r:id="rId5"/>
+    <sheet name="Scratchpad" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="CleanNumber">Number!$B$4</definedName>
-    <definedName name="Contains">Text!$B$12</definedName>
-    <definedName name="Date">Date!$B$3</definedName>
-    <definedName name="DatePlusDays">Date!$B$6</definedName>
-    <definedName name="DatePlusWorkingDays">Date!$B$7</definedName>
-    <definedName name="DateText">Date!$B$17</definedName>
-    <definedName name="Days">Date!$B$5</definedName>
-    <definedName name="FileExtension">File!$B$8</definedName>
-    <definedName name="FileName">File!$B$7</definedName>
-    <definedName name="FileNameNoExtension">File!$B$9</definedName>
-    <definedName name="FirstName">Text!$B$14</definedName>
-    <definedName name="Folder">File!$B$10</definedName>
-    <definedName name="FullFileName">File!$B$5</definedName>
-    <definedName name="Int">Number!$B$5</definedName>
-    <definedName name="LastMonthEndDate">Date!$C$12</definedName>
-    <definedName name="LastMonthStartDate">Date!$B$12</definedName>
-    <definedName name="LastName">Text!$B$15</definedName>
-    <definedName name="LastWeekFriday">Date!$C$11</definedName>
-    <definedName name="LastWeekMonday">Date!$B$11</definedName>
-    <definedName name="LastWeekSunday">Date!$D$11</definedName>
-    <definedName name="Length">Text!$B$5</definedName>
-    <definedName name="LowerCase">Text!$B$7</definedName>
-    <definedName name="Number">Number!$B$3</definedName>
-    <definedName name="NumberText">Number!$B$10</definedName>
-    <definedName name="ReformattedDate">Date!$B$28</definedName>
-    <definedName name="ReformattedFileName">File!$B$14</definedName>
-    <definedName name="ReformattedNumber">Number!$B$14</definedName>
-    <definedName name="Replace">Text!$B$10</definedName>
-    <definedName name="Result">Text!$B$11</definedName>
-    <definedName name="Search">Text!$B$9</definedName>
-    <definedName name="Text">Text!$B$3</definedName>
-    <definedName name="ThisMonthFirstWorkingDay">Date!$B$13</definedName>
-    <definedName name="ThisMonthLastWorkingDay">Date!$C$13</definedName>
-    <definedName name="Today">Date!$B$10</definedName>
-    <definedName name="Trimmed">Text!$B$4</definedName>
-    <definedName name="TwoDecimals">Number!$B$6</definedName>
-    <definedName name="UpperCase">Text!$B$6</definedName>
-    <definedName name="YYYYMMDD">Date!$B$8</definedName>
+    <definedName name="CleanNumber">Number!$B$5</definedName>
+    <definedName name="Contains">Text!$B$13</definedName>
+    <definedName name="Date_Input">Date!$B$4</definedName>
+    <definedName name="DatePlusDays">Date!$B$7</definedName>
+    <definedName name="DatePlusWorkingDays">Date!$B$8</definedName>
+    <definedName name="DateText">Date!$B$18</definedName>
+    <definedName name="Days">Date!$B$6</definedName>
+    <definedName name="FileExtension">File!$B$9</definedName>
+    <definedName name="FileName">File!$B$8</definedName>
+    <definedName name="FileNameNoExtension">File!$B$10</definedName>
+    <definedName name="FirstName">Text!$B$15</definedName>
+    <definedName name="Folder">File!$B$11</definedName>
+    <definedName name="FullFileName_Input">File!$B$6</definedName>
+    <definedName name="Int">Number!$B$6</definedName>
+    <definedName name="LastMonthEndDate">Date!$C$13</definedName>
+    <definedName name="LastMonthStartDate">Date!$B$13</definedName>
+    <definedName name="LastName">Text!$B$16</definedName>
+    <definedName name="LastWeekFriday">Date!$C$12</definedName>
+    <definedName name="LastWeekMonday">Date!$B$12</definedName>
+    <definedName name="LastWeekSunday">Date!$D$12</definedName>
+    <definedName name="Length">Text!$B$6</definedName>
+    <definedName name="LowerCase">Text!$B$8</definedName>
+    <definedName name="Number_Input">Number!$B$4</definedName>
+    <definedName name="NumberText_Input">Number!$B$11</definedName>
+    <definedName name="ReformattedDate">Date!$B$29</definedName>
+    <definedName name="ReformattedFileName">File!$B$15</definedName>
+    <definedName name="ReformattedNumber">Number!$B$15</definedName>
+    <definedName name="Replace">Text!$B$11</definedName>
+    <definedName name="Result">Text!$B$12</definedName>
+    <definedName name="Search">Text!$B$10</definedName>
+    <definedName name="Text_Input">Text!$B$4</definedName>
+    <definedName name="ThisMonthFirstWorkingDay">Date!$B$14</definedName>
+    <definedName name="ThisMonthLastWorkingDay">Date!$C$14</definedName>
+    <definedName name="Today">Date!$B$11</definedName>
+    <definedName name="Trimmed">Text!$B$5</definedName>
+    <definedName name="TwoDecimals">Number!$B$7</definedName>
+    <definedName name="UpperCase">Text!$B$7</definedName>
+    <definedName name="YYYYMMDD">Date!$B$9</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -99,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="85">
   <si>
     <t>Last month's dates (First and Last)</t>
   </si>
@@ -272,57 +273,103 @@
     <t>Folder</t>
   </si>
   <si>
+    <t>Reformatted File Name:</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>Date plus a number of days</t>
+  </si>
+  <si>
+    <t>Date plus a number of working days</t>
+  </si>
+  <si>
+    <t>Text to the left</t>
+  </si>
+  <si>
+    <t>Text to the right</t>
+  </si>
+  <si>
+    <t>Extracted text</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>John C. Doe</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>John C.</t>
+  </si>
+  <si>
+    <t>Cleaned Up</t>
+  </si>
+  <si>
+    <t>Project Notebook</t>
+  </si>
+  <si>
+    <t>- Use the cell containining the formula directly in another activity to get the value produced by your formula.</t>
+  </si>
+  <si>
+    <t>How to use the Project Notebook</t>
+  </si>
+  <si>
+    <t>How to save data</t>
+  </si>
+  <si>
+    <t>- The Project Notebook is intended for manipulating data when your automation is running. It is not intended as a place to store data.</t>
+  </si>
+  <si>
+    <t>-  To save data to an Excel file:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - If you indicate a file name that doesn't exist, it will be created when you run your project.</t>
+  </si>
+  <si>
+    <t>Formulas for working with dates</t>
+  </si>
+  <si>
+    <t>Formulas for working with text</t>
+  </si>
+  <si>
+    <t>Formulas for working with numbers</t>
+  </si>
+  <si>
+    <t>File System Helpers</t>
+  </si>
+  <si>
+    <t>Formulas for working with file names and paths</t>
+  </si>
+  <si>
+    <t>- Add a "Write Cell" activity to put the data you want to manipulate using an Excel formula into the "input cell" for your formula.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - Add a "Use Excel File" activity and choose your target Excel file.</t>
+  </si>
+  <si>
+    <t>Your Project Notebook is intended to use Excel formulas for data manipulation and calculations  It includes several samples sheets to get you started, but you have the freedom to do anything you can do in Excel.</t>
+  </si>
+  <si>
     <t>C:\temp\Untitled Document.docx</t>
-  </si>
-  <si>
-    <t>Reformatted File Name:</t>
-  </si>
-  <si>
-    <t>Days</t>
-  </si>
-  <si>
-    <t>Date plus a number of days</t>
-  </si>
-  <si>
-    <t>Date plus a number of working days</t>
-  </si>
-  <si>
-    <t>Text to the left</t>
-  </si>
-  <si>
-    <t>Text to the right</t>
-  </si>
-  <si>
-    <t>Extracted text</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>John C. Doe</t>
-  </si>
-  <si>
-    <t>Doe</t>
-  </si>
-  <si>
-    <t>John C.</t>
-  </si>
-  <si>
-    <t>Cleaned Up</t>
-  </si>
-  <si>
-    <t>File System helpers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="6">
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="###,000"/>
+    <numFmt numFmtId="165" formatCode="yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="dd\-mmm"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -351,16 +398,148 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0B744D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="72"/>
+      <color theme="0"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="17"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF0070C0"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="42"/>
+      <color theme="0"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="0"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF217346"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF339966"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00819D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -476,12 +655,172 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF339966"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF339966"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF339966"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF339966"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFF4B183"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFF4B183"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFF4B183"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFF4B183"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF339966"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF339966"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF339966"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyFill="0" applyBorder="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyProtection="0">
+      <alignment horizontal="left" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyProtection="0">
+      <alignment horizontal="left" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="5" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyProtection="0">
+      <alignment horizontal="left" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyProtection="0">
+      <alignment horizontal="left" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0"/>
+    <xf numFmtId="6" fontId="1" fillId="5" borderId="0" applyFont="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" applyNumberFormat="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="5" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="5" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -528,10 +867,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -547,13 +909,176 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="45">
+    <cellStyle name="Bottom Border" xfId="16" xr:uid="{79AD1433-2737-4ED4-9B85-92BE82D167F0}"/>
+    <cellStyle name="Bottom Green Border" xfId="17" xr:uid="{E9003193-DD9F-4D54-B68D-7574182AA968}"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma 2" xfId="44" xr:uid="{8262D58B-9960-4835-B4B0-91219CE3CFE9}"/>
+    <cellStyle name="Currency 2" xfId="40" xr:uid="{C56C1770-98D6-4A76-85B0-E047DEFE8B12}"/>
+    <cellStyle name="Currency 2 2" xfId="42" xr:uid="{6C07C4D8-79BD-467F-A57D-99C3750008CC}"/>
+    <cellStyle name="Currency 3" xfId="11" xr:uid="{69FE2FEE-EDD8-45F5-80C1-E98C476065C6}"/>
+    <cellStyle name="Date" xfId="18" xr:uid="{28983C7F-C8AB-428F-8F28-51CC52F36321}"/>
+    <cellStyle name="Date 2" xfId="39" xr:uid="{41606370-FA3B-451A-B0A4-6B4E6E39A539}"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" customBuiltin="1"/>
+    <cellStyle name="GrayCell" xfId="19" xr:uid="{5915F2CC-D46A-48C4-92DA-A6A9E94FDA36}"/>
+    <cellStyle name="GrayCell 2" xfId="30" xr:uid="{C932DE05-FB49-483F-985D-57A9ABD606BE}"/>
+    <cellStyle name="Heading 1 2" xfId="5" xr:uid="{82C3C52D-147B-4D10-8C16-36249B0EBFF3}"/>
+    <cellStyle name="Heading 1 3" xfId="12" xr:uid="{4AEABA34-9408-452D-9791-98CF9437E228}"/>
+    <cellStyle name="Heading 2 2" xfId="6" xr:uid="{C49A64C2-87DB-428F-8BE5-6F4A16C703B0}"/>
+    <cellStyle name="Heading 2 3" xfId="13" xr:uid="{30CD63F8-2D6F-4068-B49F-8E19FB4ACF74}"/>
+    <cellStyle name="Heading 3 2" xfId="29" xr:uid="{126909D3-50E4-40FC-935F-6E11ABF6544A}"/>
+    <cellStyle name="Heading 3 3" xfId="14" xr:uid="{FFA63157-1AF9-419F-82E3-01CF23A4DF92}"/>
+    <cellStyle name="Heading 4 2" xfId="15" xr:uid="{FCCBE45D-A9A8-4959-9110-165722CD1955}"/>
+    <cellStyle name="Highlight" xfId="20" xr:uid="{E8F0BE68-84F4-43BD-80A6-49D800518815}"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" customBuiltin="1"/>
+    <cellStyle name="Left Border" xfId="21" xr:uid="{752567EA-4384-43AE-B676-88EEF319FF3E}"/>
+    <cellStyle name="Left Bottom Green Border" xfId="22" xr:uid="{34B3EEC9-1AFB-46BB-BA9D-9C4050C105CA}"/>
+    <cellStyle name="Left Green Border" xfId="23" xr:uid="{D9070FD4-0ABA-471F-926C-2D88574C9CAE}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{6BC7C099-EB82-48D1-AB31-46DA4D467DA5}"/>
+    <cellStyle name="Normal 3" xfId="32" xr:uid="{B49E7D7C-2375-45E2-BFFF-FA7F5541E5F2}"/>
+    <cellStyle name="Normal 4" xfId="33" xr:uid="{9BD2CCBA-D8AD-4C17-BD02-49AAD16AC878}"/>
+    <cellStyle name="Normal 5" xfId="35" xr:uid="{DBDC21D6-3639-4234-9464-6D51CBE00719}"/>
+    <cellStyle name="Normal 5 2" xfId="38" xr:uid="{1324672F-72D6-4A22-A055-2116AF0E4D81}"/>
+    <cellStyle name="Normal 5 2 2" xfId="43" xr:uid="{0127CB7F-5661-448C-936A-C419D8F806D8}"/>
+    <cellStyle name="Normal 5 3" xfId="41" xr:uid="{82CCEA6C-B6B6-49C9-BAF0-76633DEE9C38}"/>
+    <cellStyle name="OrangeBorder" xfId="24" xr:uid="{C7E0DD48-55D3-484F-BC11-2A5937DF3881}"/>
+    <cellStyle name="OrangeBorder 2" xfId="34" xr:uid="{150FC099-82C8-4045-AA82-309796EAFE86}"/>
+    <cellStyle name="Right Bottom Green Border" xfId="25" xr:uid="{6A2C4F5A-0DDE-4C11-8235-E324DEC16A81}"/>
+    <cellStyle name="Right Green Border" xfId="26" xr:uid="{01984877-D9ED-4DDE-ACEF-8C0EE05C3CBA}"/>
+    <cellStyle name="Start Text" xfId="2" xr:uid="{EDB0B951-A110-4146-8AEC-6A70E229A2D5}"/>
+    <cellStyle name="Title 2" xfId="4" xr:uid="{FB044FE1-B1E7-4D5F-A2B7-39BD77AC425B}"/>
+    <cellStyle name="Title 3" xfId="36" xr:uid="{BAB72052-24F6-409A-A358-28D4AD66341C}"/>
+    <cellStyle name="Title 4" xfId="37" xr:uid="{BF108802-D40E-4B55-AE23-02C2EDD1EC5C}"/>
+    <cellStyle name="Title 5" xfId="8" xr:uid="{76D2112B-61B8-4476-84DD-C0B6ED5DD63F}"/>
+    <cellStyle name="Year" xfId="27" xr:uid="{875B2B43-1B18-4303-B4D5-2FCD77B5DADF}"/>
+    <cellStyle name="YellowCell" xfId="28" xr:uid="{20928AD6-9307-413A-A508-863FF7AC9DB9}"/>
+    <cellStyle name="YellowCell 2" xfId="31" xr:uid="{982BBDC1-BDF7-4E08-B354-BEA94A3EC0BF}"/>
+    <cellStyle name="z A Column text" xfId="7" xr:uid="{23B87D12-C661-428D-98E4-29837A850E3A}"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14996795556505021"/>
+          <bgColor rgb="FF217346"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="double">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9"/>
+          <bgColor rgb="FF217346"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="medium">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="medium">
+          <color theme="1"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF339966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="CustomTableStyle" pivot="0" count="2" xr9:uid="{C0886BD5-2816-460A-9ABA-29A772184C96}">
+      <tableStyleElement type="headerRow" dxfId="8"/>
+      <tableStyleElement type="firstRowStripe" dxfId="7"/>
+    </tableStyle>
+    <tableStyle name="ExcelTableStyle" pivot="0" count="7" xr9:uid="{1D1EB055-14F4-4341-8FDF-BB495A4C75BA}">
+      <tableStyleElement type="wholeTable" dxfId="6"/>
+      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="totalRow" dxfId="4"/>
+      <tableStyleElement type="firstColumn" dxfId="3"/>
+      <tableStyleElement type="lastColumn" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="FF00819D"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -563,6 +1088,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>4219069</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>18726</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F02D60CF-8928-455B-9C78-A605CA86381D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="171450" y="1876425"/>
+          <a:ext cx="4047619" cy="2590476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>4266694</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>75824</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{962976CE-2C8F-455D-A37F-D5746FB47B40}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="219075" y="5705475"/>
+          <a:ext cx="4047619" cy="3009524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -862,13 +1480,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88115396-113A-4E92-ABEE-648E1977C738}">
-  <dimension ref="D1:E5"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16" style="30" customWidth="1"/>
+    <col min="1" max="1" width="165.5546875" style="30" customWidth="1"/>
     <col min="2" max="2" width="15.44140625" style="30" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" style="30" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.44140625" style="30" bestFit="1" customWidth="1"/>
@@ -876,26 +1494,123 @@
     <col min="6" max="16384" width="8.88671875" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:5" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="36"/>
+    </row>
+    <row r="2" spans="1:5" ht="34.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A2" s="39" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="36" x14ac:dyDescent="0.3">
+      <c r="A3" s="38" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="35"/>
       <c r="D4" s="31"/>
     </row>
-    <row r="5" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="34" t="s">
+        <v>71</v>
+      </c>
       <c r="D5" s="32"/>
       <c r="E5" s="33"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="37" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="35"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="35"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="35"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="35"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="35"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="35"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="35"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="35"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="35"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="35"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="35"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="35"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="35"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="35"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="35"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="37" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="37" t="s">
+        <v>75</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53392D88-1157-4343-9701-AA198E0565D5}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -907,275 +1622,291 @@
     <col min="7" max="9" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="48" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+    </row>
+    <row r="2" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B4" s="2">
         <f ca="1">TODAY()</f>
-        <v>43868</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="25">
-        <v>7</v>
+        <v>43931</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="2">
-        <f ca="1">Date+Days</f>
-        <v>43875</v>
+        <v>58</v>
+      </c>
+      <c r="B6" s="25">
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B7" s="2">
-        <f ca="1">WORKDAY(Date, Days)</f>
-        <v>43879</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+        <f ca="1">Date_Input+Days</f>
+        <v>43938</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="2">
+        <f ca="1">WORKDAY(Date_Input, Days)</f>
+        <v>43942</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="str">
-        <f ca="1">TEXT(Date,"YYYYMMDD")</f>
-        <v>20200207</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="2">
-        <f ca="1">TODAY()</f>
-        <v>43868</v>
-      </c>
-    </row>
+      <c r="B9" t="str">
+        <f ca="1">TEXT(Date_Input,"YYYYMMDD")</f>
+        <v>20200410</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B11" s="2">
-        <f ca="1">TODAY()-WEEKDAY(TODAY(),2)-6</f>
-        <v>43857</v>
-      </c>
-      <c r="C11" s="2">
-        <f ca="1">LastWeekMonday+4</f>
-        <v>43861</v>
-      </c>
-      <c r="D11" s="2">
-        <f ca="1">LastWeekFriday+2</f>
-        <v>43863</v>
+        <f ca="1">TODAY()</f>
+        <v>43931</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B12" s="2">
-        <f ca="1">DATE(YEAR(TODAY()), MONTH(TODAY())-1, 1)</f>
-        <v>43831</v>
+        <f ca="1">TODAY()-WEEKDAY(TODAY(),2)-6</f>
+        <v>43920</v>
       </c>
       <c r="C12" s="2">
-        <f ca="1">DATE(YEAR(TODAY()), MONTH(TODAY()), 0)</f>
-        <v>43861</v>
+        <f ca="1">LastWeekMonday+4</f>
+        <v>43924</v>
+      </c>
+      <c r="D12" s="2">
+        <f ca="1">LastWeekFriday+2</f>
+        <v>43926</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="2">
+        <f ca="1">DATE(YEAR(TODAY()), MONTH(TODAY())-1, 1)</f>
+        <v>43891</v>
+      </c>
+      <c r="C13" s="2">
+        <f ca="1">DATE(YEAR(TODAY()), MONTH(TODAY()), 0)</f>
+        <v>43921</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B14" s="2">
         <f ca="1">WORKDAY(DATE(YEAR(TODAY()),MONTH(TODAY()),1)-1,1)</f>
-        <v>43864</v>
-      </c>
-      <c r="C13" s="2">
+        <v>43922</v>
+      </c>
+      <c r="C14" s="2">
         <f ca="1">WORKDAY(DATE(YEAR(TODAY()),MONTH(TODAY())+1,1),-1)</f>
-        <v>43889</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="36" t="s">
+        <v>43951</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="38"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="12" t="s">
+      <c r="B16" s="46"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="47"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="7"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="34"/>
-      <c r="D17" s="35"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="7"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>12</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B18" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="43"/>
+      <c r="D18" s="44"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B20" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="7"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="7"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="6" t="str">
-        <f>LEFT(B17, FIND(B18, B17)-1)</f>
-        <v>2008</v>
-      </c>
-      <c r="C21" s="6" t="str">
-        <f>RIGHT(B17, LEN(B17)-LEN(B21)-1)</f>
-        <v>12月31日 (水)</v>
-      </c>
-      <c r="D21" s="7" t="str">
-        <f>IF(D18&lt;&gt;"", LEFT(C21, FIND(D18, C21)-1), C21)</f>
-        <v>12月31</v>
-      </c>
+      <c r="A21" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="7"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="6" t="str">
-        <f>LEFT(C21, FIND(C18, C21)-1)</f>
-        <v>12</v>
-      </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="7"/>
+        <f>LEFT(B18, FIND(B19, B18)-1)</f>
+        <v>2008</v>
+      </c>
+      <c r="C22" s="6" t="str">
+        <f>RIGHT(B18, LEN(B18)-LEN(B22)-1)</f>
+        <v>12月31日 (水)</v>
+      </c>
+      <c r="D22" s="7" t="str">
+        <f>IF(D19&lt;&gt;"", LEFT(C22, FIND(D19, C22)-1), C22)</f>
+        <v>12月31</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="6" t="str">
-        <f>RIGHT(D21, LEN(D21)-LEN(B22)-1)</f>
-        <v>31</v>
+        <f>LEFT(C22, FIND(C19, C22)-1)</f>
+        <v>12</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="7"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="6" t="str">
+        <f>RIGHT(D22, LEN(D22)-LEN(B23)-1)</f>
         <v>31</v>
-      </c>
-      <c r="B24" s="6" t="str" cm="1">
-        <f t="array" ref="B24">_xlfn.SWITCH(FIND("Y", B19), 1, B21, 2, B22, 3, B23)</f>
-        <v>2008</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="6" t="str" cm="1">
-        <f t="array" ref="B25">_xlfn.SWITCH(FIND("M", B19), 1, B21, 2, B22, 3, B23)</f>
-        <v>12</v>
+        <f t="array" ref="B25">_xlfn.SWITCH(FIND("Y", B20), 1, B22, 2, B23, 3, B24)</f>
+        <v>2008</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="7"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" s="6" t="str" cm="1">
-        <f t="array" ref="B26">_xlfn.SWITCH(FIND("D", B19), 1, B21, 2, B22, 3, B23)</f>
-        <v>31</v>
+        <f t="array" ref="B26">_xlfn.SWITCH(FIND("M", B20), 1, B22, 2, B23, 3, B24)</f>
+        <v>12</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="7"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="6"/>
+      <c r="A27" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="6" t="str" cm="1">
+        <f t="array" ref="B27">_xlfn.SWITCH(FIND("D", B20), 1, B22, 2, B23, 3, B24)</f>
+        <v>31</v>
+      </c>
       <c r="C27" s="6"/>
       <c r="D27" s="7"/>
     </row>
-    <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="15" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="8">
-        <f>DATE(B24, B25, B26)</f>
+      <c r="B29" s="8">
+        <f>DATE(B25, B26, B27)</f>
         <v>39813</v>
       </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="10"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="A15:D15"/>
+  <mergeCells count="4">
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7C60E3-5132-4EAF-A6AE-357FE13BC6C9}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1186,203 +1917,222 @@
     <col min="6" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" s="25" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="48" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>64</v>
-      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+    </row>
+    <row r="2" spans="1:6" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" t="str">
-        <f>TRIM(B3)</f>
-        <v>John C. Doe</v>
+        <v>54</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" s="28" t="str">
-        <f>TRIM(MID(Text, FIND(D4,Text)+LEN(D4), IFERROR(FIND(IF(E4="",CHAR(10),E4),Text,FIND(D4,Text)+LEN(D4)),LEN(Text)+1)-FIND(D4,Text)-LEN(D4)))</f>
-        <v>C.</v>
+        <v>64</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5">
-        <f>LEN(B3)</f>
-        <v>11</v>
+        <v>44</v>
+      </c>
+      <c r="B5" t="str">
+        <f>TRIM(B4)</f>
+        <v>John C. Doe</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D5" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="25"/>
+      <c r="E5" s="25" t="s">
+        <v>66</v>
+      </c>
       <c r="F5" s="28" t="str">
-        <f>TRIM(MID(Text, FIND(D5,Text)+LEN(D5), IFERROR(FIND(IF(E5="",CHAR(10),E5),Text,FIND(D5,Text)+LEN(D5)),LEN(Text)+1)-FIND(D5,Text)-LEN(D5)))</f>
-        <v>C. Doe</v>
+        <f>TRIM(MID(Text_Input, FIND(D5,Text_Input)+LEN(D5), IFERROR(FIND(IF(E5="",CHAR(10),E5),Text_Input,FIND(D5,Text_Input)+LEN(D5)),LEN(Text_Input)+1)-FIND(D5,Text_Input)-LEN(D5)))</f>
+        <v>C.</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" t="str">
-        <f>UPPER(B3)</f>
-        <v>JOHN C. DOE</v>
+        <v>45</v>
+      </c>
+      <c r="B6">
+        <f>LEN(B4)</f>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25" t="s">
-        <v>67</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="25"/>
       <c r="F6" s="28" t="str">
-        <f>TRIM(MID(Text, FIND(D6,Text)+LEN(D6), IFERROR(FIND(IF(E6="",CHAR(10),E6),Text,FIND(D6,Text)+LEN(D6)),LEN(Text)+1)-FIND(D6,Text)-LEN(D6)))</f>
-        <v>John C.</v>
+        <f>TRIM(MID(Text_Input, FIND(D6,Text_Input)+LEN(D6), IFERROR(FIND(IF(E6="",CHAR(10),E6),Text_Input,FIND(D6,Text_Input)+LEN(D6)),LEN(Text_Input)+1)-FIND(D6,Text_Input)-LEN(D6)))</f>
+        <v>C. Doe</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="str">
+        <f>UPPER(B4)</f>
+        <v>JOHN C. DOE</v>
+      </c>
+      <c r="C7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="28" t="str">
+        <f>TRIM(MID(Text_Input, FIND(D7,Text_Input)+LEN(D7), IFERROR(FIND(IF(E7="",CHAR(10),E7),Text_Input,FIND(D7,Text_Input)+LEN(D7)),LEN(Text_Input)+1)-FIND(D7,Text_Input)-LEN(D7)))</f>
+        <v>John C.</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>47</v>
       </c>
-      <c r="B7" t="str">
-        <f>LOWER(B3)</f>
+      <c r="B8" t="str">
+        <f>LOWER(B4)</f>
         <v>john c. doe</v>
       </c>
-      <c r="C7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="28" t="str">
-        <f>TRIM(MID(Text, FIND(D7,Text)+LEN(D7), IFERROR(FIND(IF(E7="",CHAR(10),E7),Text,FIND(D7,Text)+LEN(D7)),LEN(Text)+1)-FIND(D7,Text)-LEN(D7)))</f>
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="25"/>
+      <c r="F8" s="28" t="str">
+        <f>TRIM(MID(Text_Input, FIND(D8,Text_Input)+LEN(D8), IFERROR(FIND(IF(E8="",CHAR(10),E8),Text_Input,FIND(D8,Text_Input)+LEN(D8)),LEN(Text_Input)+1)-FIND(D8,Text_Input)-LEN(D8)))</f>
         <v>Doe</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" s="28" t="str">
-        <f>TRIM(MID(Text, FIND(D8,Text)+LEN(D8), IFERROR(FIND(IF(E8="",CHAR(10),E8),Text,FIND(D8,Text)+LEN(D8)),LEN(Text)+1)-FIND(D8,Text)-LEN(D8)))</f>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="28" t="str">
+        <f>TRIM(MID(Text_Input, FIND(D9,Text_Input)+LEN(D9), IFERROR(FIND(IF(E9="",CHAR(10),E9),Text_Input,FIND(D9,Text_Input)+LEN(D9)),LEN(Text_Input)+1)-FIND(D9,Text_Input)-LEN(D9)))</f>
         <v>John C. Doe</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" t="str">
-        <f>SUBSTITUTE(Text, B9, B10)</f>
-        <v>Mary C. Doe</v>
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="str">
+        <f>SUBSTITUTE(Text_Input, B10, B11)</f>
+        <v>Mary C. Doe</v>
+      </c>
+      <c r="C12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>3</v>
       </c>
-      <c r="B12" t="b">
-        <f>IF(IFERROR(FIND(B9, Text), FALSE), TRUE, FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B13" t="b">
+        <f>IF(IFERROR(FIND(B10, Text), FALSE), TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" t="str">
-        <f>LEFT(Text, LEN(Text)-LEN(LastName)-1)</f>
-        <v>John C.</v>
-      </c>
       <c r="C14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" t="str">
+        <f>LEFT(Text_Input, LEN(Text_Input)-LEN(LastName)-1)</f>
+        <v>John C.</v>
+      </c>
+      <c r="C15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>52</v>
       </c>
-      <c r="B15" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(B3," ",REPT(" ",LEN(B3))),LEN(B3)))</f>
+      <c r="B16" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(B4," ",REPT(" ",LEN(B4))),LEN(B4)))</f>
         <v>Doe</v>
       </c>
-      <c r="C15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1390,9 +2140,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C83CC8-3284-4752-8E92-8CBBD1003835}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1402,102 +2154,121 @@
     <col min="5" max="5" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="48" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="49"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+    </row>
+    <row r="3" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="40"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="29">
+      <c r="B4" s="29">
         <v>3.1415929999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="B4" s="25">
-        <f>VALUE(TRIM(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(Number, CHAR(13), ""), CHAR(10), ""), CHAR(160), "")))</f>
+    <row r="5" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="25">
+        <f>VALUE(TRIM(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(Number_Input, CHAR(13), ""), CHAR(10), ""), CHAR(160), "")))</f>
         <v>3.1415929999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>38</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <f>INT(CleanNumber)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>39</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <f>INT(CleanNumber*100)/100</f>
         <v>3.14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="36" t="s">
+    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="38"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
+      <c r="B9" s="47"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="7"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>6</v>
-      </c>
+      <c r="B10" s="7"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="4"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B13" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="7"/>
-    </row>
-    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="15" t="s">
+      <c r="B14" s="7"/>
+    </row>
+    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="11">
-        <f>IF(B11&lt;&gt;"",IF(B12&lt;&gt;"",_xlfn.NUMBERVALUE(B10, B11, B12),_xlfn.NUMBERVALUE(B10, B11)),IF(B12&lt;&gt;"",_xlfn.NUMBERVALUE(B10,, B12),_xlfn.NUMBERVALUE(B10)))</f>
+      <c r="B15" s="11">
+        <f>IF(B12&lt;&gt;"",IF(B13&lt;&gt;"",_xlfn.NUMBERVALUE(B11, B12, B13),_xlfn.NUMBERVALUE(B11, B12)),IF(B13&lt;&gt;"",_xlfn.NUMBERVALUE(B11,, B13),_xlfn.NUMBERVALUE(B11)))</f>
         <v>123456.78</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A8:B8"/>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A9:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1506,10 +2277,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B15AA95-D2AA-4AD6-8E83-DBFAD20B8498}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1519,87 +2290,121 @@
     <col min="3" max="4" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="36" t="s">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+    </row>
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="49"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+    </row>
+    <row r="3" spans="1:4" s="42" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="40"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="38"/>
-    </row>
-    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="27" t="s">
+      <c r="B4" s="47"/>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="26"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
+      <c r="B5" s="26"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B6" s="22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="17"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="17" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(B6,"\",REPT(" ",LEN(B6))),LEN(B6)))</f>
+        <v>Untitled Document.docx</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="17" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(B8,".",REPT(" ",LEN(B8))),LEN(B8)))</f>
+        <v>docx</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="17" t="str">
+        <f>LEFT(B8, LEN(B8)-LEN(B9)-1)</f>
+        <v>Untitled Document</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="18" t="str">
+        <f>LEFT(B6, LEN(B6)-LEN(B8))</f>
+        <v>C:\temp\</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="17"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="17" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(B5,"\",REPT(" ",LEN(B5))),LEN(B5)))</f>
-        <v>Untitled Document.docx</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="17" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(B7,".",REPT(" ",LEN(B7))),LEN(B7)))</f>
-        <v>docx</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="17" t="str">
-        <f>LEFT(B7, LEN(B7)-LEN(B8)-1)</f>
-        <v>Untitled Document</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="18" t="str">
-        <f>LEFT(B5, LEN(B5)-LEN(B7))</f>
-        <v>C:\temp\</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="B14" s="25" t="str">
+      <c r="B15" s="25" t="str">
         <f>FileNameNoExtension &amp; "." &amp; FileExtension</f>
         <v>Untitled Document.docx</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A3:B3"/>
+  <mergeCells count="3">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95188A8B-20B9-44C0-8B2D-2363D0E3925F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>